<commit_message>
Remembering all the triage data points
</commit_message>
<xml_diff>
--- a/RR ongoing questions.xlsx
+++ b/RR ongoing questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CS_Knit_tinK_SC\Documents\GitProjects\FinTech-BC-Final-IndStudy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58E6C07-F556-4D2A-B339-161103251658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F0D419-5537-4602-8847-35C6B97C7EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15915" yWindow="885" windowWidth="11940" windowHeight="13335" xr2:uid="{C0F82931-DCB6-43BA-9323-F577D148C00E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Ongoing RR questions</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>Do any NOC reports need to be requsted today?</t>
+  </si>
+  <si>
+    <t>Are there any new FASB rulings to get up to speed on?</t>
+  </si>
+  <si>
+    <t>Did any bank statements (not online ones) arrive in mail today?</t>
   </si>
 </sst>
 </file>
@@ -430,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70E19FEC-BC53-4C9F-A4AE-18052A61D50A}">
-  <dimension ref="B2:D24"/>
+  <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,6 +506,16 @@
         <v>11</v>
       </c>
     </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>